<commit_message>
Update poison scroll color
</commit_message>
<xml_diff>
--- a/rogue-boi-core/assets/game-config.xlsx
+++ b/rogue-boi-core/assets/game-config.xlsx
@@ -276,7 +276,7 @@
     <t xml:space="preserve">Poison the enemy</t>
   </si>
   <si>
-    <t xml:space="preserve">green</t>
+    <t xml:space="preserve">#84f437</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -721,7 +721,7 @@
       <c r="O1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="0"/>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -1198,7 +1198,7 @@
       <c r="M20" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="N20" s="0" t="n">
+      <c r="N20" s="3" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add rare weapons to level 3
</commit_message>
<xml_diff>
--- a/rogue-boi-core/assets/game-config.xlsx
+++ b/rogue-boi-core/assets/game-config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="enemy-chances" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="93">
   <si>
     <t xml:space="preserve">level</t>
   </si>
@@ -78,6 +78,12 @@
     <t xml:space="preserve">PoisonScroll</t>
   </si>
   <si>
+    <t xml:space="preserve">RareSword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RareDagger</t>
+  </si>
+  <si>
     <t xml:space="preserve">icon</t>
   </si>
   <si>
@@ -286,6 +292,15 @@
   </si>
   <si>
     <t xml:space="preserve">#84f437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rare Sword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#0d09ed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rare Dagger</t>
   </si>
 </sst>
 </file>
@@ -408,7 +423,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="6:6 A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -528,10 +543,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="6:6 E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -648,6 +663,28 @@
       </c>
       <c r="C10" s="2" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -666,10 +703,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="6:6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -689,89 +726,89 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>10</v>
@@ -788,27 +825,27 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -816,16 +853,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>100</v>
@@ -848,16 +885,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>35</v>
@@ -880,17 +917,17 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D9" s="2" t="str">
         <f aca="false">"Comfy armor, adding "&amp;J9&amp;" defense"</f>
         <v>Comfy armor, adding 1 defense</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J9" s="2" t="n">
         <v>1</v>
@@ -901,16 +938,16 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="J10" s="2" t="n">
         <v>3</v>
@@ -921,17 +958,17 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2" t="str">
         <f aca="false">"Larger weapon dealing "&amp;H11&amp;" damage"</f>
         <v>Larger weapon dealing 4 damage</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>4</v>
@@ -945,17 +982,17 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D12" s="2" t="str">
         <f aca="false">"Small weapon dealing "&amp;H12&amp;" damage"</f>
         <v>Small weapon dealing 2 damage</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>2</v>
@@ -969,17 +1006,17 @@
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D13" s="2" t="str">
         <f aca="false">"Restores "&amp;K13&amp;" health"</f>
         <v>Restores 3 health</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>3</v>
@@ -990,16 +1027,16 @@
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L14" s="2" t="n">
         <v>3</v>
@@ -1016,16 +1053,16 @@
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L15" s="2" t="n">
         <v>10</v>
@@ -1042,17 +1079,17 @@
         <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D16" s="2" t="str">
         <f aca="false">"Hurl a fireball dealing damage in an area with radius "&amp;O16&amp;" for "&amp;L16&amp;" damage"</f>
         <v>Hurl a fireball dealing damage in an area with radius 3 for 4 damage</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L16" s="2" t="n">
         <v>4</v>
@@ -1072,16 +1109,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>200</v>
@@ -1104,16 +1141,16 @@
         <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>25</v>
@@ -1136,16 +1173,16 @@
         <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F19" s="2" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F7*2/3)+5</f>
@@ -1172,16 +1209,16 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>120</v>
@@ -1204,16 +1241,16 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="L21" s="2" t="n">
         <v>1</v>
@@ -1224,6 +1261,61 @@
       <c r="N21" s="3" t="n">
         <v>4</v>
       </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f aca="false">"Rare sword dealing "&amp;H22&amp;" damage"</f>
+        <v>Rare sword dealing 7 damage</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f aca="false">"Rare dagger dealing "&amp;H23&amp;" damage"</f>
+        <v>Rare dagger dealing 5 damage</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="2" t="n">
+        <f aca="false">_xlfn.FLOOR.MATH((H22+H11)/2)</f>
+        <v>5</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J25" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat: Add zombie enemy
</commit_message>
<xml_diff>
--- a/rogue-boi-core/assets/game-config.xlsx
+++ b/rogue-boi-core/assets/game-config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="enemy-chances" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="97">
   <si>
     <t xml:space="preserve">level</t>
   </si>
@@ -51,6 +51,9 @@
     <t xml:space="preserve">Minotaur</t>
   </si>
   <si>
+    <t xml:space="preserve">Zombie</t>
+  </si>
+  <si>
     <t xml:space="preserve">HpPotion</t>
   </si>
   <si>
@@ -301,6 +304,15 @@
   </si>
   <si>
     <t xml:space="preserve">Rare Dagger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zombie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shambling corpse. Once belonged to an adventurer like  you</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#f0ddd7</t>
   </si>
 </sst>
 </file>
@@ -420,13 +432,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -441,7 +453,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -452,7 +464,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -474,7 +486,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -485,7 +497,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -496,7 +508,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -507,7 +519,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
@@ -518,13 +530,24 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -545,11 +568,11 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="5.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="14.43"/>
@@ -571,7 +594,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>80</v>
@@ -582,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>40</v>
@@ -593,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>40</v>
@@ -604,7 +627,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>10</v>
@@ -615,7 +638,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>30</v>
@@ -626,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>30</v>
@@ -637,7 +660,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>25</v>
@@ -648,7 +671,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>25</v>
@@ -659,7 +682,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>10</v>
@@ -670,9 +693,9 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="n">
         <v>10</v>
       </c>
     </row>
@@ -681,9 +704,9 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="n">
         <v>15</v>
       </c>
     </row>
@@ -706,10 +729,10 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="13.34"/>
@@ -718,7 +741,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="13.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="13.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="13.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="13.45"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,89 +749,89 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G4" s="2" t="n">
         <v>10</v>
@@ -825,27 +848,27 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,16 +876,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>100</v>
@@ -885,16 +908,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>35</v>
@@ -914,20 +937,20 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9" s="2" t="str">
         <f aca="false">"Comfy armor, adding "&amp;J9&amp;" defense"</f>
         <v>Comfy armor, adding 1 defense</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J9" s="2" t="n">
         <v>1</v>
@@ -935,19 +958,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="J10" s="2" t="n">
         <v>3</v>
@@ -955,20 +978,20 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D11" s="2" t="str">
         <f aca="false">"Larger weapon dealing "&amp;H11&amp;" damage"</f>
         <v>Larger weapon dealing 4 damage</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H11" s="2" t="n">
         <v>4</v>
@@ -979,20 +1002,20 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" s="2" t="str">
         <f aca="false">"Small weapon dealing "&amp;H12&amp;" damage"</f>
         <v>Small weapon dealing 2 damage</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H12" s="2" t="n">
         <v>2</v>
@@ -1003,20 +1026,20 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2" t="str">
         <f aca="false">"Restores "&amp;K13&amp;" health"</f>
         <v>Restores 3 health</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K13" s="2" t="n">
         <v>3</v>
@@ -1024,19 +1047,19 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L14" s="2" t="n">
         <v>3</v>
@@ -1050,19 +1073,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L15" s="2" t="n">
         <v>10</v>
@@ -1076,20 +1099,20 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D16" s="2" t="str">
         <f aca="false">"Hurl a fireball dealing damage in an area with radius "&amp;O16&amp;" for "&amp;L16&amp;" damage"</f>
         <v>Hurl a fireball dealing damage in an area with radius 3 for 4 damage</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L16" s="2" t="n">
         <v>4</v>
@@ -1109,16 +1132,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>200</v>
@@ -1141,16 +1164,16 @@
         <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>25</v>
@@ -1173,16 +1196,16 @@
         <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F19" s="2" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F7*2/3)+5</f>
@@ -1209,16 +1232,16 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>120</v>
@@ -1238,19 +1261,19 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L21" s="2" t="n">
         <v>1</v>
@@ -1264,20 +1287,20 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D22" s="2" t="str">
         <f aca="false">"Rare sword dealing "&amp;H22&amp;" damage"</f>
         <v>Rare sword dealing 7 damage</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H22" s="2" t="n">
         <v>7</v>
@@ -1288,20 +1311,20 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D23" s="2" t="str">
         <f aca="false">"Rare dagger dealing "&amp;H23&amp;" damage"</f>
         <v>Rare dagger dealing 5 damage</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H23" s="2" t="n">
         <f aca="false">_xlfn.FLOOR.MATH((H22+H11)/2)</f>
@@ -1312,7 +1335,36 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G24" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J25" s="2"/>

</xml_diff>

<commit_message>
Add validator to game-config
</commit_message>
<xml_diff>
--- a/rogue-boi-core/assets/game-config.xlsx
+++ b/rogue-boi-core/assets/game-config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
   <si>
     <t xml:space="preserve">level</t>
   </si>
@@ -432,10 +432,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -521,7 +521,7 @@
       <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="3" t="n">
@@ -540,17 +540,34 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="3" t="n">
         <v>30</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B1011" type="list">
+      <formula1>'stuff-descriptor'!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -569,7 +586,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -711,6 +728,12 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B1012" type="list">
+      <formula1>'stuff-descriptor'!$A$2:$A$1048576</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -729,7 +752,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
balance: Lower zombie melee skill. Update some descriptions
</commit_message>
<xml_diff>
--- a/rogue-boi-core/assets/game-config.xlsx
+++ b/rogue-boi-core/assets/game-config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="103">
   <si>
     <t xml:space="preserve">tag</t>
   </si>
@@ -93,6 +93,9 @@
     <t xml:space="preserve">person</t>
   </si>
   <si>
+    <t xml:space="preserve">Your very self</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wall</t>
   </si>
   <si>
@@ -141,6 +144,9 @@
     <t xml:space="preserve">Leather Vest</t>
   </si>
   <si>
+    <t xml:space="preserve">Comfy armor</t>
+  </si>
+  <si>
     <t xml:space="preserve">#00BFFF</t>
   </si>
   <si>
@@ -165,6 +171,9 @@
     <t xml:space="preserve">Simple Sword</t>
   </si>
   <si>
+    <t xml:space="preserve">Larger weapon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dagger</t>
   </si>
   <si>
@@ -174,6 +183,9 @@
     <t xml:space="preserve">Simple Dagger</t>
   </si>
   <si>
+    <t xml:space="preserve">Small weapon</t>
+  </si>
+  <si>
     <t xml:space="preserve">HpPotion</t>
   </si>
   <si>
@@ -288,6 +300,9 @@
     <t xml:space="preserve">Rare Sword</t>
   </si>
   <si>
+    <t xml:space="preserve">Rare sword formally owned by a knight</t>
+  </si>
+  <si>
     <t xml:space="preserve">#0d09ed</t>
   </si>
   <si>
@@ -295,6 +310,9 @@
   </si>
   <si>
     <t xml:space="preserve">Rare Dagger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rare dagger</t>
   </si>
   <si>
     <t xml:space="preserve">Zombie</t>
@@ -541,7 +559,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -642,6 +660,9 @@
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
@@ -660,41 +681,41 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>18</v>
@@ -717,19 +738,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>35</v>
@@ -749,20 +770,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="1" t="str">
-        <f aca="false">"Comfy armor, adding "&amp;J9&amp;" defense"</f>
-        <v>Comfy armor, adding 1 defense</v>
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J9" s="1" t="n">
         <v>1</v>
@@ -770,19 +790,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="J10" s="1" t="n">
         <v>3</v>
@@ -790,20 +810,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="1" t="str">
-        <f aca="false">"Larger weapon dealing "&amp;H11&amp;" damage"</f>
-        <v>Larger weapon dealing 4 damage</v>
+        <v>48</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>4</v>
@@ -814,20 +833,19 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="1" t="str">
-        <f aca="false">"Small weapon dealing "&amp;H12&amp;" damage"</f>
-        <v>Small weapon dealing 2 damage</v>
+        <v>52</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>2</v>
@@ -838,20 +856,20 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D13" s="1" t="str">
         <f aca="false">"Restores "&amp;K13&amp;" health"</f>
         <v>Restores 3 health</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>3</v>
@@ -859,19 +877,19 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="L14" s="1" t="n">
         <v>3</v>
@@ -885,19 +903,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L15" s="1" t="n">
         <v>10</v>
@@ -911,20 +929,20 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1" t="str">
         <f aca="false">"Hurl a fireball dealing damage in an area with radius "&amp;O16&amp;" for "&amp;L16&amp;" damage"</f>
         <v>Hurl a fireball dealing damage in an area with radius 3 for 4 damage</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L16" s="1" t="n">
         <v>4</v>
@@ -941,19 +959,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>200</v>
@@ -973,19 +991,19 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>25</v>
@@ -1005,19 +1023,19 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F7*2/3)+5</f>
@@ -1041,19 +1059,19 @@
     </row>
     <row r="20" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>120</v>
@@ -1073,19 +1091,19 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="L21" s="1" t="n">
         <v>1</v>
@@ -1099,20 +1117,19 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="1" t="str">
-        <f aca="false">"Rare sword dealing "&amp;H22&amp;" damage"</f>
-        <v>Rare sword dealing 7 damage</v>
+        <v>91</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>7</v>
@@ -1123,20 +1140,19 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="1" t="str">
-        <f aca="false">"Rare dagger dealing "&amp;H23&amp;" damage"</f>
-        <v>Rare dagger dealing 5 damage</v>
+        <v>95</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H23" s="1" t="n">
         <f aca="false">_xlfn.FLOOR.MATH((H22+H11)/2)</f>
@@ -1148,19 +1164,19 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="F24" s="1" t="n">
         <v>50</v>
@@ -1172,7 +1188,7 @@
         <v>3</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J24" s="1" t="n">
         <v>1</v>
@@ -1207,13 +1223,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1221,7 +1237,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>80</v>
@@ -1232,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>120</v>
@@ -1243,7 +1259,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>15</v>
@@ -1254,7 +1270,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>30</v>
@@ -1265,7 +1281,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>30</v>
@@ -1276,7 +1292,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>60</v>
@@ -1287,7 +1303,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>80</v>
@@ -1298,7 +1314,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>50</v>
@@ -1309,7 +1325,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>30</v>
@@ -1320,7 +1336,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>80</v>
@@ -1362,13 +1378,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1376,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>80</v>
@@ -1387,7 +1403,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>40</v>
@@ -1398,7 +1414,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>40</v>
@@ -1409,7 +1425,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>10</v>
@@ -1420,7 +1436,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>30</v>
@@ -1431,7 +1447,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>30</v>
@@ -1442,7 +1458,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>25</v>
@@ -1453,7 +1469,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>25</v>
@@ -1464,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>10</v>
@@ -1475,7 +1491,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>10</v>
@@ -1486,7 +1502,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>15</v>

</xml_diff>

<commit_message>
feat: Add Scroll of Warding
Prevents damage for X instances
</commit_message>
<xml_diff>
--- a/rogue-boi-core/assets/game-config.xlsx
+++ b/rogue-boi-core/assets/game-config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="stuff-descriptor" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="107">
   <si>
     <t xml:space="preserve">tag</t>
   </si>
@@ -325,6 +325,18 @@
   </si>
   <si>
     <t xml:space="preserve">#f0ddd7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WardScroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scroll of Warding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cast a spell of warding on yourself.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#12cbe3</t>
   </si>
   <si>
     <t xml:space="preserve">level</t>
@@ -558,8 +570,8 @@
   </sheetPr>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1195,7 +1207,31 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="J25" s="1"/>
+      <c r="L25" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1223,13 +1259,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,10 +1400,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1378,13 +1414,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,9 +1544,31 @@
         <v>15</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B1012" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B12 B15:B1012" type="list">
       <formula1>'stuff-descriptor'!$A$2:$A$1048576</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Paving the way for different room types
</commit_message>
<xml_diff>
--- a/rogue-boi-core/assets/game-config.xlsx
+++ b/rogue-boi-core/assets/game-config.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="stuff-descriptor" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="enemy-chances" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="item-chances" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="room-chances" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="111">
   <si>
     <t xml:space="preserve">tag</t>
   </si>
@@ -343,6 +344,18 @@
   </si>
   <si>
     <t xml:space="preserve">weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal</t>
   </si>
 </sst>
 </file>
@@ -424,7 +437,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -443,6 +456,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -574,7 +591,7 @@
       <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.34"/>
@@ -1069,7 +1086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>82</v>
       </c>
@@ -1226,10 +1243,10 @@
       <c r="L25" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="M25" s="0" t="n">
+      <c r="M25" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="N25" s="0" t="n">
+      <c r="N25" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1255,7 +1272,7 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1402,11 +1419,11 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.43"/>
@@ -1551,7 +1568,7 @@
       <c r="B13" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="3" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1562,7 +1579,7 @@
       <c r="B14" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="3" t="n">
         <v>20</v>
       </c>
     </row>
@@ -1581,4 +1598,58 @@
     <oddFooter>&amp;C&amp;"Nimbus Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Value to items
</commit_message>
<xml_diff>
--- a/rogue-boi-core/assets/game-config.xlsx
+++ b/rogue-boi-core/assets/game-config.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="114">
   <si>
     <t xml:space="preserve">tag</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">aoe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
   </si>
   <si>
     <t xml:space="preserve">Stairs</t>
@@ -456,12 +459,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -590,7 +593,9 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <pane xSplit="1" ySplit="0" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="P26" activeCellId="0" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -651,51 +656,53 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3"/>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>10</v>
@@ -712,44 +719,44 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>100</v>
@@ -769,19 +776,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>35</v>
@@ -801,59 +808,65 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J9" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="P9" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="J10" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="P10" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>4</v>
@@ -861,22 +874,25 @@
       <c r="I11" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="P11" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>2</v>
@@ -884,43 +900,49 @@
       <c r="I12" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="P12" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13" s="1" t="str">
         <f aca="false">"Restores "&amp;K13&amp;" health"</f>
         <v>Restores 3 health</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K13" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="P13" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L14" s="1" t="n">
         <v>3</v>
@@ -931,22 +953,25 @@
       <c r="N14" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="P14" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L15" s="1" t="n">
         <v>10</v>
@@ -957,23 +982,26 @@
       <c r="N15" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="P15" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" s="1" t="str">
         <f aca="false">"Hurl a fireball dealing damage in an area with radius "&amp;O16&amp;" for "&amp;L16&amp;" damage"</f>
         <v>Hurl a fireball dealing damage in an area with radius 3 for 4 damage</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L16" s="1" t="n">
         <v>4</v>
@@ -987,22 +1015,25 @@
       <c r="O16" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="P16" s="0" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>200</v>
@@ -1022,19 +1053,19 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>25</v>
@@ -1054,19 +1085,19 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>80</v>
+      <c r="D19" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">_xlfn.CEILING.MATH(F7*2/3)+5</f>
@@ -1090,19 +1121,19 @@
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>84</v>
+      <c r="D20" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>120</v>
@@ -1122,19 +1153,19 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L21" s="1" t="n">
         <v>1</v>
@@ -1142,25 +1173,28 @@
       <c r="M21" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="N21" s="3" t="n">
+      <c r="N21" s="4" t="n">
         <v>4</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H22" s="1" t="n">
         <v>7</v>
@@ -1168,22 +1202,25 @@
       <c r="I22" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="P22" s="0" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H23" s="1" t="n">
         <f aca="false">_xlfn.FLOOR.MATH((H22+H11)/2)</f>
@@ -1192,22 +1229,25 @@
       <c r="I23" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="P23" s="0" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="D24" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F24" s="1" t="n">
         <v>50</v>
@@ -1227,60 +1267,63 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J25" s="1"/>
       <c r="L25" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="M25" s="3" t="n">
+      <c r="M25" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="N25" s="3" t="n">
+      <c r="N25" s="4" t="n">
         <v>0</v>
+      </c>
+      <c r="P25" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="F26" s="4" t="n">
         <v>500</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="4" t="n">
         <v>5000</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="I26" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="J26" s="0" t="n">
+      <c r="J26" s="4" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -1310,13 +1353,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,7 +1367,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>80</v>
@@ -1335,7 +1378,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>120</v>
@@ -1346,7 +1389,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>15</v>
@@ -1357,7 +1400,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>30</v>
@@ -1368,7 +1411,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>30</v>
@@ -1379,20 +1422,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="4" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="C8" s="4" t="n">
         <v>80</v>
       </c>
     </row>
@@ -1401,31 +1444,31 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="3" t="n">
+        <v>98</v>
+      </c>
+      <c r="C10" s="4" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="3" t="n">
+        <v>76</v>
+      </c>
+      <c r="C11" s="4" t="n">
         <v>80</v>
       </c>
     </row>
@@ -1465,13 +1508,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1479,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>80</v>
@@ -1490,7 +1533,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>40</v>
@@ -1501,7 +1544,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>40</v>
@@ -1512,7 +1555,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>10</v>
@@ -1523,7 +1566,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>30</v>
@@ -1534,7 +1577,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>30</v>
@@ -1545,7 +1588,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>25</v>
@@ -1556,7 +1599,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>25</v>
@@ -1567,7 +1610,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>10</v>
@@ -1578,9 +1621,9 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="3" t="n">
+        <v>91</v>
+      </c>
+      <c r="C11" s="4" t="n">
         <v>10</v>
       </c>
     </row>
@@ -1589,9 +1632,9 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="C12" s="4" t="n">
         <v>15</v>
       </c>
     </row>
@@ -1600,9 +1643,9 @@
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="3" t="n">
+        <v>102</v>
+      </c>
+      <c r="C13" s="4" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1611,9 +1654,9 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="3" t="n">
+        <v>102</v>
+      </c>
+      <c r="C14" s="4" t="n">
         <v>20</v>
       </c>
     </row>
@@ -1649,31 +1692,31 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" s="3" t="n">
+      <c r="A2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="3" t="n">
+      <c r="A3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="4" t="n">
         <v>90</v>
       </c>
     </row>

</xml_diff>